<commit_message>
Updating project to Python >= 3.6
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -1,35 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BMPxlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DD844-25DF-4B85-A055-81F6C36533A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="28680" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>tss</t>
+  </si>
+  <si>
+    <t>tn</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,15 +64,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,107 +381,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="D1" t="n">
-        <v>13.4</v>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>tss</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>47.8</v>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>tn</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>tp</t>
-        </is>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="D1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D6" sqref="D1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="D1" t="n">
-        <v>23.4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="D2" t="n">
-        <v>57.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="D1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="D1" t="n">
-        <v>33.4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="D2" t="n">
-        <v>67.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated README, build is passing on Python >= 3.6.
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BMPxlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DD844-25DF-4B85-A055-81F6C36533A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D296F8DD-3D55-419A-91D1-FA6A15B9AB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>tss</t>
-  </si>
-  <si>
-    <t>tn</t>
-  </si>
-  <si>
-    <t>tp</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,30 +372,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -415,7 +387,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D1:D6"/>
+      <selection activeCell="E7" sqref="C1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="C1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>